<commit_message>
New version from Robert
</commit_message>
<xml_diff>
--- a/inputs/AddictO_Defs.xlsx
+++ b/inputs/AddictO_Defs.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9293" uniqueCount="3595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9294" uniqueCount="3596">
   <si>
     <t>ID</t>
   </si>
@@ -10832,6 +10832,9 @@
   </si>
   <si>
     <t>******</t>
+  </si>
+  <si>
+    <t>*******</t>
   </si>
 </sst>
 </file>
@@ -11444,7 +11447,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A281" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A285" sqref="A285"/>
+      <selection pane="bottomLeft" activeCell="C286" sqref="C286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19149,7 +19152,9 @@
       <c r="R283" s="11"/>
     </row>
     <row r="284" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A284" s="11"/>
+      <c r="A284" s="11" t="s">
+        <v>3595</v>
+      </c>
       <c r="B284" s="11" t="s">
         <v>1664</v>
       </c>

</xml_diff>